<commit_message>
replace heading keys with custom labels
</commit_message>
<xml_diff>
--- a/example/example.xlsx
+++ b/example/example.xlsx
@@ -372,11 +372,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:H3"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>parent1.child1.child11</v>
+        <v>First grandchild</v>
       </c>
       <c r="B1" t="str">
         <v>parent1.child1.child12</v>
@@ -394,22 +394,10 @@
         <v>parent2.child1.child21</v>
       </c>
       <c r="G1" t="str">
-        <v>parent1.child2.child21</v>
+        <v>parent1.child3.child31</v>
       </c>
       <c r="H1" t="str">
-        <v>parent1.child2.child22</v>
-      </c>
-      <c r="I1" t="str">
-        <v>parent1.child3.child31</v>
-      </c>
-      <c r="J1" t="str">
         <v>parent1.child3.child32</v>
-      </c>
-      <c r="K1" t="str">
-        <v>parent2.child1.child11</v>
-      </c>
-      <c r="L1" t="str">
-        <v>parent2.child1.child21</v>
       </c>
     </row>
     <row r="2">
@@ -431,18 +419,6 @@
       <c r="F2">
         <v>102</v>
       </c>
-      <c r="G2">
-        <v>20</v>
-      </c>
-      <c r="H2">
-        <v>21</v>
-      </c>
-      <c r="K2">
-        <v>101</v>
-      </c>
-      <c r="L2">
-        <v>102</v>
-      </c>
     </row>
     <row r="3">
       <c r="C3">
@@ -458,22 +434,10 @@
         <v>102</v>
       </c>
       <c r="G3">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H3">
-        <v>21</v>
-      </c>
-      <c r="I3">
-        <v>30</v>
-      </c>
-      <c r="J3">
         <v>31</v>
-      </c>
-      <c r="K3">
-        <v>101</v>
-      </c>
-      <c r="L3">
-        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
options object instead of parameters
</commit_message>
<xml_diff>
--- a/example/example.xlsx
+++ b/example/example.xlsx
@@ -379,25 +379,25 @@
         <v>First grandchild</v>
       </c>
       <c r="B1" t="str">
-        <v>parent1.child1.child12</v>
+        <v>parent1-child1-child12</v>
       </c>
       <c r="C1" t="str">
-        <v>parent1.child2.child21</v>
+        <v>parent1-child2-child21</v>
       </c>
       <c r="D1" t="str">
-        <v>parent1.child2.child22</v>
+        <v>parent1-child2-child22</v>
       </c>
       <c r="E1" t="str">
-        <v>parent2.child1.child11</v>
+        <v>parent2-child1-child11</v>
       </c>
       <c r="F1" t="str">
-        <v>parent2.child1.child21</v>
+        <v>parent2-child1-child21</v>
       </c>
       <c r="G1" t="str">
-        <v>parent1.child3.child31</v>
+        <v>parent1-child3-child31</v>
       </c>
       <c r="H1" t="str">
-        <v>parent1.child3.child32</v>
+        <v>parent1-child3-child32</v>
       </c>
     </row>
     <row r="2">

</xml_diff>